<commit_message>
Created Analyser for giving basic analysis of product reviews
</commit_message>
<xml_diff>
--- a/reviews.xlsx
+++ b/reviews.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Review</t>
+  </si>
+  <si>
+    <t>Stars</t>
   </si>
   <si>
     <t>Chris</t>
@@ -467,114 +470,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>